<commit_message>
forgotten edits caught in inspection
</commit_message>
<xml_diff>
--- a/pyOurPubs/results/papers_postprocess.xlsx
+++ b/pyOurPubs/results/papers_postprocess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/grad_utils/pyOurPubs/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CCBF3D-ABCA-B242-AFE4-9611B95CCA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702004EB-8EEA-3B43-91E7-717F751AB511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="23600" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="2000" windowWidth="27400" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>pmid</t>
   </si>
   <si>
-    <t>Katrina Lee</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Eric</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>36094401</t>
+  </si>
+  <si>
+    <t>Katrina</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H12" sqref="B2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -675,6 +675,8 @@
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -705,25 +707,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -731,25 +733,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -757,25 +759,25 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -783,25 +785,25 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -809,25 +811,25 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -835,51 +837,51 @@
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -887,25 +889,25 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -913,30 +915,30 @@
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -945,7 +947,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>45</v>
@@ -965,25 +967,25 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -999,6 +1001,9 @@
       <c r="A16" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
+    <sortCondition ref="G2:G12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>